<commit_message>
nettoyage GHI, jointure GHI2000>2021 et GHI2022, gestion des valeurs manquantes par interpolation
</commit_message>
<xml_diff>
--- a/GHI 2022-version2.xlsx
+++ b/GHI 2022-version2.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3757a171cf8daaf/Bureau/Faim dans le monde_hunger_in_the_world/dataset GHI global hunger index/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d3757a171cf8daaf/Bureau/GHI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{78651B1E-0D46-4484-9ED1-1A24C8D45E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="14_{78651B1E-0D46-4484-9ED1-1A24C8D45E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BBE43F1-AE82-4136-B2B3-347E3F3F699F}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-885" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau 1" sheetId="1" r:id="rId1"/>
     <sheet name="Tableau 1_1" sheetId="2" r:id="rId2"/>
     <sheet name="Tableau 1_2" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Tableau 1'!$A$1:$C$130</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -561,7 +564,7 @@
       <name val="ArialMT"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -578,6 +581,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -684,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -732,6 +741,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,6 +825,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,13 +1130,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
     <col min="2" max="2" width="16.6328125" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" customWidth="1"/>
     <col min="4" max="4" width="26.26953125" customWidth="1"/>
@@ -1155,7 +1169,7 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="22" t="s">
@@ -1337,7 +1351,7 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="23" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -1506,7 +1520,7 @@
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B30" s="1">
@@ -1727,7 +1741,7 @@
       <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="20" customHeight="1">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="23" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="1">
@@ -1831,7 +1845,7 @@
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5" ht="20" customHeight="1">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="23" t="s">
         <v>57</v>
       </c>
       <c r="B55" s="1">
@@ -1922,7 +1936,7 @@
       <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:5" ht="20" customHeight="1">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="23" t="s">
         <v>64</v>
       </c>
       <c r="B62" s="1">
@@ -2091,7 +2105,7 @@
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" ht="20" customHeight="1">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="23" t="s">
         <v>77</v>
       </c>
       <c r="B75" s="1">
@@ -2234,7 +2248,7 @@
       <c r="E85" s="1"/>
     </row>
     <row r="86" spans="1:5" ht="20" customHeight="1">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="23" t="s">
         <v>88</v>
       </c>
       <c r="B86" s="1">
@@ -2364,7 +2378,7 @@
       <c r="E95" s="1"/>
     </row>
     <row r="96" spans="1:5" ht="20" customHeight="1">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="23" t="s">
         <v>98</v>
       </c>
       <c r="B96" s="1">
@@ -2390,7 +2404,7 @@
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5" ht="20" customHeight="1">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="23" t="s">
         <v>100</v>
       </c>
       <c r="B98" s="1">
@@ -2494,7 +2508,7 @@
       <c r="E105" s="1"/>
     </row>
     <row r="106" spans="1:5" ht="20" customHeight="1">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="23" t="s">
         <v>108</v>
       </c>
       <c r="B106" s="1">
@@ -2559,7 +2573,7 @@
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5" ht="20" customHeight="1">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="23" t="s">
         <v>113</v>
       </c>
       <c r="B111" s="1">
@@ -2572,7 +2586,7 @@
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5" ht="20" customHeight="1">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="23" t="s">
         <v>114</v>
       </c>
       <c r="B112" s="1">
@@ -2585,7 +2599,7 @@
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5" ht="20" customHeight="1">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="23" t="s">
         <v>115</v>
       </c>
       <c r="B113" s="1">
@@ -2715,7 +2729,7 @@
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5" ht="20" customHeight="1">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="23" t="s">
         <v>127</v>
       </c>
       <c r="B123" s="21">
@@ -2741,7 +2755,7 @@
       <c r="E124" s="1"/>
     </row>
     <row r="125" spans="1:5" ht="20" customHeight="1">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="23" t="s">
         <v>129</v>
       </c>
       <c r="B125" s="21">
@@ -2806,7 +2820,7 @@
       <c r="E129" s="1"/>
     </row>
     <row r="130" spans="1:5" ht="20" customHeight="1">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="23" t="s">
         <v>135</v>
       </c>
       <c r="B130" s="3" t="s">
@@ -2819,6 +2833,7 @@
       <c r="E130" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C130" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>